<commit_message>
Keep close HEAD requests to ES
</commit_message>
<xml_diff>
--- a/datapackage_pipelines_budgetkey/pipelines/budget/national/processed/budget_conversions.xlsx
+++ b/datapackage_pipelines_budgetkey/pipelines/budget/national/processed/budget_conversions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Code/obudget/budgetkey-data-pipelines/datapackage_pipelines_budgetkey/pipelines/budget/national/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56F021C-1FF6-7148-8F19-1900CAFC1C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B585C9F3-5F6A-2148-8187-C52F7E53DAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7653,7 +7653,7 @@
   <dimension ref="A1:C1210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1048576"/>
+      <selection activeCell="C1" sqref="C1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>